<commit_message>
added NKK M2028TJW01-GA-1A  - the brake bias toggle switch that the DRS MCU is built around - to the BOM
</commit_message>
<xml_diff>
--- a/hardware/DAQ-PDU AIO Rev 2 PCB Files/DAQ-PDU AIO Rev 2 BOM.xlsx
+++ b/hardware/DAQ-PDU AIO Rev 2 PCB Files/DAQ-PDU AIO Rev 2 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_sav\Desktop\School and Work (post Aug'18)\Formula SAE Stuff\DAQ-PDU AIO Board\DAQ Rev 2 PCB Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_sav\Desktop\SchoolandWork\Formula SAE Stuff\DAQ-PDU AIO Board\hardware\DAQ-PDU AIO Rev 2 PCB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66A037D-D574-4E89-B65E-916F763ECB80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C17FCA3-F001-44D9-A6C3-9C7962FEFF95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAQ-PDU AIO Rev 2 BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>Mfr No.</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/NKK-Switches/M2028TJW01-GA-1A?qs=HrqAcaC9xK5l%252BLLRcEF4FQ%3D%3D</t>
+  </si>
+  <si>
+    <t>M2028TJW01-GA-1A</t>
+  </si>
+  <si>
+    <t>Brake Bias Toggle Switch (NKK Switches)</t>
   </si>
 </sst>
 </file>
@@ -1125,20 +1134,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="37.21875" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
-    <col min="6" max="7" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.20703125" customWidth="1"/>
+    <col min="5" max="5" width="24.7890625" customWidth="1"/>
+    <col min="6" max="7" width="21.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1232,7 +1241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1272,7 +1281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1437,7 +1446,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1508,7 +1517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1546,6 +1555,17 @@
       </c>
       <c r="F22" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed sensor in bom from 150U to 050B
</commit_message>
<xml_diff>
--- a/hardware/DAQ-PDU AIO Rev 2 PCB Files/DAQ-PDU AIO Rev 2 BOM.xlsx
+++ b/hardware/DAQ-PDU AIO Rev 2 PCB Files/DAQ-PDU AIO Rev 2 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_sav\Desktop\SchoolandWork\Formula SAE Stuff\DAQ-PDU AIO Board\hardware\DAQ-PDU AIO Rev 2 PCB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C17FCA3-F001-44D9-A6C3-9C7962FEFF95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA9677F-5EEA-4727-B76F-35A4755E08A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,18 +91,9 @@
     <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0805W8F1001T5E_C17513.html</t>
   </si>
   <si>
-    <t>ACS781 Current Sensor</t>
-  </si>
-  <si>
     <t>U10, U14, U66, U68, U84, U87, U103, U108, U109, U113, U116, U121, U128, U131, U150</t>
   </si>
   <si>
-    <t xml:space="preserve">ACS781KLRTR-150B-T </t>
-  </si>
-  <si>
-    <t>https://www.arrow.com/en/products/acs781klrtr-150b-t/allegro-microsystems</t>
-  </si>
-  <si>
     <t>0.1uF Cap SMD Ceramic</t>
   </si>
   <si>
@@ -269,6 +260,15 @@
   </si>
   <si>
     <t>Brake Bias Toggle Switch (NKK Switches)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACS781KLRTR-050B-T </t>
+  </si>
+  <si>
+    <t>ACS781 50A bidirectional Current Sensor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/allegro-microsystems/ACS781LLRTR-050B-T/6189096</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1161,7 +1161,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1266,19 +1266,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
       </c>
       <c r="D7">
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1286,19 +1286,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1306,19 +1306,19 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1326,16 +1326,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1343,19 +1343,19 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1363,19 +1363,19 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1383,16 +1383,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1400,16 +1400,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1417,16 +1417,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1434,16 +1434,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1451,16 +1451,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1468,10 +1468,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1482,19 +1482,19 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1502,19 +1502,19 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1522,19 +1522,19 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1542,37 +1542,34 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" xr:uid="{EAD6C956-261B-4023-98FB-F47E177087C2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>